<commit_message>
NX Get Measurements Updates
Added two significant features to `nx_get_measurements.py`:
1) Export metadata in JSON along with measurements. Metadata includes
part name, revision, extraction date, user, and part units.
2) Support for points, vectors, strings, and list expression types.
These are now included in the JSON that's exported; however, there is no
implementation for them elsewhere in DATUM at this time. In addition to
this, the WCS feature is also exported, in order to give reference for
the MOI and POI that come out of mass measurements.

Updated xlpnr to change `expr["type"]` to `expr["description"]` since
`Expression.Type` is already used in the NX API (returns Point, Vector,
Number, etc.) and "description" now points to the end of the string that
tells us that this is a radius, mass, surface normal, etc.
</commit_message>
<xml_diff>
--- a/tests/xl/datum_excel_tests.xlsx
+++ b/tests/xl/datum_excel_tests.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25128"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20385"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\blair\datum\tests\xl\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\frandeen\Documents\datum\tests\xl\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F6112C4D-D8D3-443E-8F91-A029D316B6F1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F022A443-E15A-4B16-86C5-846625504A9C}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="768" yWindow="768" windowWidth="17280" windowHeight="9960" firstSheet="1" activeTab="1" xr2:uid="{4E3D2296-B548-4056-9C4B-8EF4E130383B}"/>
+    <workbookView xWindow="770" yWindow="770" windowWidth="17280" windowHeight="9960" firstSheet="1" activeTab="1" xr2:uid="{4E3D2296-B548-4056-9C4B-8EF4E130383B}"/>
   </bookViews>
   <sheets>
     <sheet name="Other Tests" sheetId="3" r:id="rId1"/>
@@ -37,16 +37,6 @@
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
@@ -491,20 +481,20 @@
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.90625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="8.88671875" style="1"/>
-    <col min="2" max="2" width="26.77734375" style="1" customWidth="1"/>
-    <col min="3" max="16384" width="8.88671875" style="1"/>
+    <col min="1" max="1" width="8.90625" style="1"/>
+    <col min="2" max="2" width="26.81640625" style="1" customWidth="1"/>
+    <col min="3" max="16384" width="8.90625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" s="3" t="s">
         <v>18</v>
       </c>
       <c r="B1" s="3"/>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
         <v>14</v>
       </c>
@@ -512,7 +502,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
         <v>15</v>
       </c>
@@ -520,7 +510,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A4" s="1" t="s">
         <v>16</v>
       </c>
@@ -528,7 +518,7 @@
         <v>3.1415190000000002</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A5" s="1" t="s">
         <v>17</v>
       </c>
@@ -553,25 +543,25 @@
       <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.90625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="9.5546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="23.88671875" style="1" customWidth="1"/>
-    <col min="3" max="16384" width="8.88671875" style="1"/>
+    <col min="1" max="1" width="9.54296875" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="23.90625" style="1" customWidth="1"/>
+    <col min="3" max="16384" width="8.90625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A3" s="2"/>
       <c r="B3" s="1" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
       <c r="B4" s="1" t="s">
         <v>2</v>
       </c>
@@ -582,7 +572,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
       <c r="B5" s="1" t="s">
         <v>3</v>
       </c>
@@ -593,7 +583,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
       <c r="B6" s="1" t="s">
         <v>4</v>
       </c>
@@ -604,7 +594,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.35">
       <c r="B7" s="1" t="s">
         <v>5</v>
       </c>
@@ -615,7 +605,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.35">
       <c r="B8" s="1" t="s">
         <v>6</v>
       </c>
@@ -626,7 +616,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.35">
       <c r="B9" s="1" t="s">
         <v>7</v>
       </c>
@@ -634,7 +624,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.35">
       <c r="B10" s="1" t="s">
         <v>8</v>
       </c>

</xml_diff>

<commit_message>
added list index capability (MOI, POI, etc.)
</commit_message>
<xml_diff>
--- a/tests/xl/datum_excel_tests.xlsx
+++ b/tests/xl/datum_excel_tests.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\frandeen\Documents\datum\tests\xl\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BC3CD76B-D004-48F5-81E7-B76614A6FA80}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{87C6A7EF-BDE4-45A2-8449-897652906AB8}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="770" yWindow="770" windowWidth="17280" windowHeight="9960" firstSheet="1" activeTab="1" xr2:uid="{4E3D2296-B548-4056-9C4B-8EF4E130383B}"/>
   </bookViews>
@@ -17,15 +17,22 @@
     <sheet name="Gearbox Tests" sheetId="1" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="AIR_NUT">'Gearbox Tests'!$C$9</definedName>
+    <definedName name="AIR_NUT.point">'Gearbox Tests'!$C$9:$E$9</definedName>
     <definedName name="Date_range">'Gearbox Tests'!$A$3</definedName>
-    <definedName name="DIPSTICK">'Gearbox Tests'!$C$8</definedName>
+    <definedName name="DIPSTICK.angle">'Gearbox Tests'!$C$8</definedName>
     <definedName name="FASTENERS.mass">'Gearbox Tests'!$C$6</definedName>
     <definedName name="float_range">'Gearbox Tests'!$A$2</definedName>
     <definedName name="GEARS.mass">'Gearbox Tests'!$C$7</definedName>
     <definedName name="HOUSING.mass">'Gearbox Tests'!$C$5</definedName>
+    <definedName name="HOUSING.moments_of_inertia_centroidal.0">'Gearbox Tests'!$C$17</definedName>
+    <definedName name="HOUSING.moments_of_inertia_centroidal.1">'Gearbox Tests'!$C$18</definedName>
+    <definedName name="HOUSING.moments_of_inertia_centroidal.2">'Gearbox Tests'!$C$19</definedName>
     <definedName name="missing_ref">'Other Tests'!#REF!</definedName>
     <definedName name="SHAFT_CENTERS">'Gearbox Tests'!$C$10</definedName>
+    <definedName name="SHAFT_CENTERS.distance">'Gearbox Tests'!$C$10</definedName>
+    <definedName name="SHAFT_CENTERS.point_1.x">'Gearbox Tests'!$C$11</definedName>
+    <definedName name="SHAFT_CENTERS.point_1.y">'Gearbox Tests'!$C$12</definedName>
+    <definedName name="SHAFT_CENTERS.point_1.z">'Gearbox Tests'!$C$13</definedName>
     <definedName name="SURFACE_PAINTED.area">'Gearbox Tests'!$C$4</definedName>
     <definedName name="Test_Date">'Other Tests'!$B$5</definedName>
     <definedName name="Test_Float">'Other Tests'!$B$4</definedName>
@@ -43,7 +50,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="26">
   <si>
     <t>Because spreadsheets need dark mode too!</t>
   </si>
@@ -100,6 +107,27 @@
   </si>
   <si>
     <t>TEST VALUES -- DO NOT MODIFY</t>
+  </si>
+  <si>
+    <t>x</t>
+  </si>
+  <si>
+    <t>y</t>
+  </si>
+  <si>
+    <t>z</t>
+  </si>
+  <si>
+    <t>HOUSING MOI</t>
+  </si>
+  <si>
+    <t>MXX</t>
+  </si>
+  <si>
+    <t>MYY</t>
+  </si>
+  <si>
+    <t>MZZ</t>
   </si>
 </sst>
 </file>
@@ -537,10 +565,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{54907CF9-C14B-4766-B22F-13A5988C480B}">
-  <dimension ref="A1:D10"/>
+  <dimension ref="A1:E19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.90625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -550,18 +578,18 @@
     <col min="3" max="16384" width="8.90625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A3" s="2"/>
       <c r="B3" s="1" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
       <c r="B4" s="1" t="s">
         <v>2</v>
       </c>
@@ -572,7 +600,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
       <c r="B5" s="1" t="s">
         <v>3</v>
       </c>
@@ -583,7 +611,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
       <c r="B6" s="1" t="s">
         <v>4</v>
       </c>
@@ -594,7 +622,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
       <c r="B7" s="1" t="s">
         <v>5</v>
       </c>
@@ -605,7 +633,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
       <c r="B8" s="1" t="s">
         <v>6</v>
       </c>
@@ -616,23 +644,82 @@
         <v>11</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.35">
       <c r="B9" s="1" t="s">
         <v>7</v>
       </c>
       <c r="C9" s="1">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.35">
+        <v>1</v>
+      </c>
+      <c r="D9" s="1">
+        <v>2</v>
+      </c>
+      <c r="E9" s="1">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.35">
       <c r="B10" s="1" t="s">
         <v>8</v>
       </c>
       <c r="C10" s="1">
-        <v>7</v>
+        <v>159.99999999999989</v>
       </c>
       <c r="D10" s="1" t="s">
         <v>12</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="B11" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C11" s="1">
+        <v>899.99999999999909</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="B12" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C12" s="1">
+        <v>865.63897914069571</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="B13" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C13" s="1">
+        <v>261.00000000000006</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="B16" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="17" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B17" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C17" s="1">
+        <v>2734036.863510197</v>
+      </c>
+    </row>
+    <row r="18" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B18" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C18" s="1">
+        <v>3833609.1842077454</v>
+      </c>
+    </row>
+    <row r="19" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B19" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C19" s="1">
+        <v>4349785.7993760025</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Read & Write Vector Capability
Added capability to XLPNR to read from and write to ranges of more than
one cell, primarily for writing row or column matrices, which from NX
measurements arise from lists (MOI, POI, etc.), vectors, and points.

Capability to call out a single coordinate (MEAUREMENT.point.x) for a
single cell, or a range (MEASUREMENT.point) which would be a 1x3 or 3x1
arrangement.

Updated unit tests; coverage not complete. Working.
</commit_message>
<xml_diff>
--- a/tests/xl/datum_excel_tests.xlsx
+++ b/tests/xl/datum_excel_tests.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\frandeen\Documents\datum\tests\xl\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{87C6A7EF-BDE4-45A2-8449-897652906AB8}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{00C7790D-1014-4A94-BE5B-B2504361BB45}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="770" yWindow="770" windowWidth="17280" windowHeight="9960" firstSheet="1" activeTab="1" xr2:uid="{4E3D2296-B548-4056-9C4B-8EF4E130383B}"/>
   </bookViews>
@@ -24,9 +24,11 @@
     <definedName name="float_range">'Gearbox Tests'!$A$2</definedName>
     <definedName name="GEARS.mass">'Gearbox Tests'!$C$7</definedName>
     <definedName name="HOUSING.mass">'Gearbox Tests'!$C$5</definedName>
+    <definedName name="HOUSING.moments_of_inertia_centroidal">'Gearbox Tests'!$C$17:$C$19</definedName>
     <definedName name="HOUSING.moments_of_inertia_centroidal.0">'Gearbox Tests'!$C$17</definedName>
     <definedName name="HOUSING.moments_of_inertia_centroidal.1">'Gearbox Tests'!$C$18</definedName>
     <definedName name="HOUSING.moments_of_inertia_centroidal.2">'Gearbox Tests'!$C$19</definedName>
+    <definedName name="HOUSING.products_of_inertia_centroidal">'Gearbox Tests'!$C$22:$C$24</definedName>
     <definedName name="missing_ref">'Other Tests'!#REF!</definedName>
     <definedName name="SHAFT_CENTERS">'Gearbox Tests'!$C$10</definedName>
     <definedName name="SHAFT_CENTERS.distance">'Gearbox Tests'!$C$10</definedName>
@@ -50,7 +52,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="30">
   <si>
     <t>Because spreadsheets need dark mode too!</t>
   </si>
@@ -128,6 +130,18 @@
   </si>
   <si>
     <t>MZZ</t>
+  </si>
+  <si>
+    <t>HOUSING POI</t>
+  </si>
+  <si>
+    <t>PXY</t>
+  </si>
+  <si>
+    <t>PXZ</t>
+  </si>
+  <si>
+    <t>PYZ</t>
   </si>
 </sst>
 </file>
@@ -565,10 +579,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{54907CF9-C14B-4766-B22F-13A5988C480B}">
-  <dimension ref="A1:E19"/>
+  <dimension ref="A1:E24"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+    <sheetView tabSelected="1" topLeftCell="A3" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="C22" sqref="C22:C24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.90625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -649,13 +663,13 @@
         <v>7</v>
       </c>
       <c r="C9" s="1">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="D9" s="1">
-        <v>2</v>
+        <v>2.11</v>
       </c>
       <c r="E9" s="1">
-        <v>3</v>
+        <v>9.99</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.35">
@@ -698,28 +712,57 @@
         <v>22</v>
       </c>
     </row>
-    <row r="17" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="17" spans="2:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B17" s="1" t="s">
         <v>23</v>
       </c>
       <c r="C17" s="1">
-        <v>2734036.863510197</v>
-      </c>
-    </row>
-    <row r="18" spans="2:3" x14ac:dyDescent="0.35">
+        <v>1.2E-2</v>
+      </c>
+    </row>
+    <row r="18" spans="2:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B18" s="1" t="s">
         <v>24</v>
       </c>
       <c r="C18" s="1">
-        <v>3833609.1842077454</v>
-      </c>
-    </row>
-    <row r="19" spans="2:3" x14ac:dyDescent="0.35">
+        <v>0.11</v>
+      </c>
+    </row>
+    <row r="19" spans="2:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B19" s="1" t="s">
         <v>25</v>
       </c>
       <c r="C19" s="1">
-        <v>4349785.7993760025</v>
+        <v>0.99</v>
+      </c>
+    </row>
+    <row r="21" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B21" s="1" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="22" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B22" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="C22" s="1">
+        <v>-8350.6714059345395</v>
+      </c>
+    </row>
+    <row r="23" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B23" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="C23" s="1">
+        <v>-48498.809284873329</v>
+      </c>
+    </row>
+    <row r="24" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B24" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="C24" s="1">
+        <v>26209.492442448263</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
build: restructure as module
Add __init__.py to datum subfolder. Add folder for nx_journals and
organize that folder.
</commit_message>
<xml_diff>
--- a/tests/xl/datum_excel_tests.xlsx
+++ b/tests/xl/datum_excel_tests.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20385"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25128"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\frandeen\Documents\datum\tests\xl\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\blair\datum\tests\xl\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{00C7790D-1014-4A94-BE5B-B2504361BB45}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F572912A-A15B-4DEC-AADF-688CF9223D2A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="770" yWindow="770" windowWidth="17280" windowHeight="9960" firstSheet="1" activeTab="1" xr2:uid="{4E3D2296-B548-4056-9C4B-8EF4E130383B}"/>
+    <workbookView xWindow="768" yWindow="768" windowWidth="17280" windowHeight="9960" firstSheet="1" activeTab="1" xr2:uid="{4E3D2296-B548-4056-9C4B-8EF4E130383B}"/>
   </bookViews>
   <sheets>
     <sheet name="Other Tests" sheetId="3" r:id="rId1"/>
@@ -523,20 +523,20 @@
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.90625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="8.90625" style="1"/>
-    <col min="2" max="2" width="26.81640625" style="1" customWidth="1"/>
-    <col min="3" max="16384" width="8.90625" style="1"/>
+    <col min="1" max="1" width="8.88671875" style="1"/>
+    <col min="2" max="2" width="26.77734375" style="1" customWidth="1"/>
+    <col min="3" max="16384" width="8.88671875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
         <v>18</v>
       </c>
       <c r="B1" s="3"/>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>14</v>
       </c>
@@ -544,7 +544,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>15</v>
       </c>
@@ -552,7 +552,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
         <v>16</v>
       </c>
@@ -560,7 +560,7 @@
         <v>3.1415190000000002</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
         <v>17</v>
       </c>
@@ -585,25 +585,25 @@
       <selection activeCell="C22" sqref="C22:C24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.90625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="9.54296875" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="23.90625" style="1" customWidth="1"/>
-    <col min="3" max="16384" width="8.90625" style="1"/>
+    <col min="1" max="1" width="9.5546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="23.88671875" style="1" customWidth="1"/>
+    <col min="3" max="16384" width="8.88671875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" s="2"/>
       <c r="B3" s="1" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B4" s="1" t="s">
         <v>2</v>
       </c>
@@ -614,7 +614,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B5" s="1" t="s">
         <v>3</v>
       </c>
@@ -625,7 +625,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B6" s="1" t="s">
         <v>4</v>
       </c>
@@ -636,7 +636,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B7" s="1" t="s">
         <v>5</v>
       </c>
@@ -647,7 +647,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B8" s="1" t="s">
         <v>6</v>
       </c>
@@ -658,7 +658,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B9" s="1" t="s">
         <v>7</v>
       </c>
@@ -672,7 +672,7 @@
         <v>9.99</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B10" s="1" t="s">
         <v>8</v>
       </c>
@@ -683,7 +683,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B11" s="1" t="s">
         <v>19</v>
       </c>
@@ -691,7 +691,7 @@
         <v>899.99999999999909</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B12" s="1" t="s">
         <v>20</v>
       </c>
@@ -699,7 +699,7 @@
         <v>865.63897914069571</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B13" s="1" t="s">
         <v>21</v>
       </c>
@@ -707,12 +707,12 @@
         <v>261.00000000000006</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B16" s="1" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="17" spans="2:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="17" spans="2:3" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B17" s="1" t="s">
         <v>23</v>
       </c>
@@ -720,7 +720,7 @@
         <v>1.2E-2</v>
       </c>
     </row>
-    <row r="18" spans="2:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="18" spans="2:3" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B18" s="1" t="s">
         <v>24</v>
       </c>
@@ -728,7 +728,7 @@
         <v>0.11</v>
       </c>
     </row>
-    <row r="19" spans="2:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="19" spans="2:3" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B19" s="1" t="s">
         <v>25</v>
       </c>
@@ -736,12 +736,12 @@
         <v>0.99</v>
       </c>
     </row>
-    <row r="21" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="21" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B21" s="1" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="22" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="22" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B22" s="1" t="s">
         <v>27</v>
       </c>
@@ -749,7 +749,7 @@
         <v>-8350.6714059345395</v>
       </c>
     </row>
-    <row r="23" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="23" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B23" s="1" t="s">
         <v>28</v>
       </c>
@@ -757,7 +757,7 @@
         <v>-48498.809284873329</v>
       </c>
     </row>
-    <row r="24" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="24" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B24" s="1" t="s">
         <v>29</v>
       </c>

</xml_diff>

<commit_message>
feat: improved logging & test logging
Updated xlpnr.py to use __name__ rather than "root". Updated
logging.conf to add a test logger. Test logger keeps error messages out
of the console (they are expected, no need to write them out) and writes
them to a separate file, in a slightly different format. Minor changes
in console & test file to accommodate.
</commit_message>
<xml_diff>
--- a/tests/xl/datum_excel_tests.xlsx
+++ b/tests/xl/datum_excel_tests.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25128"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20385"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\blair\datum\tests\xl\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\frandeen\Documents\datum\tests\xl\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F572912A-A15B-4DEC-AADF-688CF9223D2A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5A79811C-DE01-4F77-AD28-A1B22D277B4C}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="768" yWindow="768" windowWidth="17280" windowHeight="9960" firstSheet="1" activeTab="1" xr2:uid="{4E3D2296-B548-4056-9C4B-8EF4E130383B}"/>
+    <workbookView xWindow="770" yWindow="770" windowWidth="17280" windowHeight="9960" firstSheet="1" activeTab="1" xr2:uid="{4E3D2296-B548-4056-9C4B-8EF4E130383B}"/>
   </bookViews>
   <sheets>
     <sheet name="Other Tests" sheetId="3" r:id="rId1"/>
@@ -523,20 +523,20 @@
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.90625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="8.88671875" style="1"/>
-    <col min="2" max="2" width="26.77734375" style="1" customWidth="1"/>
-    <col min="3" max="16384" width="8.88671875" style="1"/>
+    <col min="1" max="1" width="8.90625" style="1"/>
+    <col min="2" max="2" width="26.81640625" style="1" customWidth="1"/>
+    <col min="3" max="16384" width="8.90625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" s="3" t="s">
         <v>18</v>
       </c>
       <c r="B1" s="3"/>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
         <v>14</v>
       </c>
@@ -544,7 +544,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
         <v>15</v>
       </c>
@@ -552,7 +552,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A4" s="1" t="s">
         <v>16</v>
       </c>
@@ -560,7 +560,7 @@
         <v>3.1415190000000002</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A5" s="1" t="s">
         <v>17</v>
       </c>
@@ -585,25 +585,25 @@
       <selection activeCell="C22" sqref="C22:C24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.90625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="9.5546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="23.88671875" style="1" customWidth="1"/>
-    <col min="3" max="16384" width="8.88671875" style="1"/>
+    <col min="1" max="1" width="9.54296875" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="23.90625" style="1" customWidth="1"/>
+    <col min="3" max="16384" width="8.90625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A3" s="2"/>
       <c r="B3" s="1" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
       <c r="B4" s="1" t="s">
         <v>2</v>
       </c>
@@ -614,7 +614,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
       <c r="B5" s="1" t="s">
         <v>3</v>
       </c>
@@ -625,7 +625,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
       <c r="B6" s="1" t="s">
         <v>4</v>
       </c>
@@ -636,7 +636,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
       <c r="B7" s="1" t="s">
         <v>5</v>
       </c>
@@ -647,7 +647,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
       <c r="B8" s="1" t="s">
         <v>6</v>
       </c>
@@ -658,7 +658,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.35">
       <c r="B9" s="1" t="s">
         <v>7</v>
       </c>
@@ -672,7 +672,7 @@
         <v>9.99</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.35">
       <c r="B10" s="1" t="s">
         <v>8</v>
       </c>
@@ -683,7 +683,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.35">
       <c r="B11" s="1" t="s">
         <v>19</v>
       </c>
@@ -691,7 +691,7 @@
         <v>899.99999999999909</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.35">
       <c r="B12" s="1" t="s">
         <v>20</v>
       </c>
@@ -699,7 +699,7 @@
         <v>865.63897914069571</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.35">
       <c r="B13" s="1" t="s">
         <v>21</v>
       </c>
@@ -707,12 +707,12 @@
         <v>261.00000000000006</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.35">
       <c r="B16" s="1" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="17" spans="2:3" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="2:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B17" s="1" t="s">
         <v>23</v>
       </c>
@@ -720,7 +720,7 @@
         <v>1.2E-2</v>
       </c>
     </row>
-    <row r="18" spans="2:3" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="2:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B18" s="1" t="s">
         <v>24</v>
       </c>
@@ -728,7 +728,7 @@
         <v>0.11</v>
       </c>
     </row>
-    <row r="19" spans="2:3" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="2:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B19" s="1" t="s">
         <v>25</v>
       </c>
@@ -736,12 +736,12 @@
         <v>0.99</v>
       </c>
     </row>
-    <row r="21" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="21" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B21" s="1" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="22" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="22" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B22" s="1" t="s">
         <v>27</v>
       </c>
@@ -749,7 +749,7 @@
         <v>-8350.6714059345395</v>
       </c>
     </row>
-    <row r="23" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="23" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B23" s="1" t="s">
         <v>28</v>
       </c>
@@ -757,7 +757,7 @@
         <v>-48498.809284873329</v>
       </c>
     </row>
-    <row r="24" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="24" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B24" s="1" t="s">
         <v>29</v>
       </c>

</xml_diff>

<commit_message>
feat: preview of lists and dicts.
</commit_message>
<xml_diff>
--- a/tests/xl/datum_excel_tests.xlsx
+++ b/tests/xl/datum_excel_tests.xlsx
@@ -1,23 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20385"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25128"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\frandeen\Documents\datum\tests\xl\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\blair\datum\tests\xl\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5A79811C-DE01-4F77-AD28-A1B22D277B4C}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{09B6C5CF-F936-4A31-AAB2-BB5AAC1A1C2E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="770" yWindow="770" windowWidth="17280" windowHeight="9960" firstSheet="1" activeTab="1" xr2:uid="{4E3D2296-B548-4056-9C4B-8EF4E130383B}"/>
+    <workbookView xWindow="2304" yWindow="2304" windowWidth="17280" windowHeight="9960" firstSheet="1" activeTab="1" xr2:uid="{4E3D2296-B548-4056-9C4B-8EF4E130383B}"/>
   </bookViews>
   <sheets>
     <sheet name="Other Tests" sheetId="3" r:id="rId1"/>
     <sheet name="Gearbox Tests" sheetId="1" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="AIR_NUT.point">'Gearbox Tests'!$C$9:$E$9</definedName>
+    <definedName name="AIR_NUT.point_1">'Gearbox Tests'!$C$9:$E$9</definedName>
     <definedName name="Date_range">'Gearbox Tests'!$A$3</definedName>
     <definedName name="DIPSTICK.angle">'Gearbox Tests'!$C$8</definedName>
     <definedName name="FASTENERS.mass">'Gearbox Tests'!$C$6</definedName>
@@ -52,7 +52,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="29">
   <si>
     <t>Because spreadsheets need dark mode too!</t>
   </si>
@@ -88,9 +88,6 @@
   </si>
   <si>
     <t>deg</t>
-  </si>
-  <si>
-    <t>mm</t>
   </si>
   <si>
     <t>Kivo is a dork</t>
@@ -523,46 +520,46 @@
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.90625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="8.90625" style="1"/>
-    <col min="2" max="2" width="26.81640625" style="1" customWidth="1"/>
-    <col min="3" max="16384" width="8.90625" style="1"/>
+    <col min="1" max="1" width="8.88671875" style="1"/>
+    <col min="2" max="2" width="26.77734375" style="1" customWidth="1"/>
+    <col min="3" max="16384" width="8.88671875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B1" s="3"/>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B2" s="1">
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A4" s="1" t="s">
         <v>15</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A4" s="1" t="s">
-        <v>16</v>
       </c>
       <c r="B4" s="1">
         <v>3.1415190000000002</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B5" s="2">
         <v>44682</v>
@@ -581,29 +578,29 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{54907CF9-C14B-4766-B22F-13A5988C480B}">
   <dimension ref="A1:E24"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="C22" sqref="C22:C24"/>
+    <sheetView tabSelected="1" topLeftCell="A6" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.90625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="9.54296875" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="23.90625" style="1" customWidth="1"/>
-    <col min="3" max="16384" width="8.90625" style="1"/>
+    <col min="1" max="1" width="9.5546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="23.88671875" style="1" customWidth="1"/>
+    <col min="3" max="16384" width="8.88671875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" s="2"/>
       <c r="B3" s="1" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B4" s="1" t="s">
         <v>2</v>
       </c>
@@ -614,7 +611,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B5" s="1" t="s">
         <v>3</v>
       </c>
@@ -625,7 +622,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B6" s="1" t="s">
         <v>4</v>
       </c>
@@ -636,29 +633,29 @@
         <v>10</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B7" s="1" t="s">
         <v>5</v>
       </c>
       <c r="C7" s="1">
-        <v>54.455593060061851</v>
+        <v>45</v>
       </c>
       <c r="D7" s="1" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B8" s="1" t="s">
         <v>6</v>
       </c>
       <c r="C8" s="1">
-        <v>90</v>
+        <v>95</v>
       </c>
       <c r="D8" s="1" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B9" s="1" t="s">
         <v>7</v>
       </c>
@@ -672,94 +669,97 @@
         <v>9.99</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B10" s="1" t="s">
         <v>8</v>
       </c>
       <c r="C10" s="1">
         <v>159.99999999999989</v>
       </c>
-      <c r="D10" s="1" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="D10" s="1">
+        <v>925.99999999999989</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B11" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C11" s="1">
+        <v>0</v>
+      </c>
+      <c r="D11" s="1">
+        <v>439.08443537387728</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="B12" s="1" t="s">
         <v>19</v>
-      </c>
-      <c r="C11" s="1">
-        <v>899.99999999999909</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="B12" s="1" t="s">
-        <v>20</v>
       </c>
       <c r="C12" s="1">
         <v>865.63897914069571</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B13" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C13" s="1">
         <v>261.00000000000006</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B16" s="1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="17" spans="2:3" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B17" s="1" t="s">
         <v>22</v>
-      </c>
-    </row>
-    <row r="17" spans="2:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B17" s="1" t="s">
-        <v>23</v>
       </c>
       <c r="C17" s="1">
         <v>1.2E-2</v>
       </c>
     </row>
-    <row r="18" spans="2:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="18" spans="2:3" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B18" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C18" s="1">
         <v>0.11</v>
       </c>
     </row>
-    <row r="19" spans="2:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="19" spans="2:3" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B19" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C19" s="1">
         <v>0.99</v>
       </c>
     </row>
-    <row r="21" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="21" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B21" s="1" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="22" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B22" s="1" t="s">
         <v>26</v>
-      </c>
-    </row>
-    <row r="22" spans="2:3" x14ac:dyDescent="0.35">
-      <c r="B22" s="1" t="s">
-        <v>27</v>
       </c>
       <c r="C22" s="1">
         <v>-8350.6714059345395</v>
       </c>
     </row>
-    <row r="23" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="23" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B23" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C23" s="1">
         <v>-48498.809284873329</v>
       </c>
     </row>
-    <row r="24" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="24" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B24" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C24" s="1">
         <v>26209.492442448263</v>

</xml_diff>

<commit_message>
style: black, flake8, isort
Also switch venv to python 3.8.3, update .gitignore
</commit_message>
<xml_diff>
--- a/tests/xl/datum_excel_tests.xlsx
+++ b/tests/xl/datum_excel_tests.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\blair\datum\tests\xl\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{09B6C5CF-F936-4A31-AAB2-BB5AAC1A1C2E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E7500AC3-68E3-4ADD-9BC0-67893599017E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2304" yWindow="2304" windowWidth="17280" windowHeight="9960" firstSheet="1" activeTab="1" xr2:uid="{4E3D2296-B548-4056-9C4B-8EF4E130383B}"/>
+    <workbookView xWindow="3040" yWindow="3040" windowWidth="28800" windowHeight="15410" firstSheet="1" activeTab="1" xr2:uid="{4E3D2296-B548-4056-9C4B-8EF4E130383B}"/>
   </bookViews>
   <sheets>
     <sheet name="Other Tests" sheetId="3" r:id="rId1"/>
@@ -520,20 +520,20 @@
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.90625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="8.88671875" style="1"/>
-    <col min="2" max="2" width="26.77734375" style="1" customWidth="1"/>
-    <col min="3" max="16384" width="8.88671875" style="1"/>
+    <col min="1" max="1" width="8.90625" style="1"/>
+    <col min="2" max="2" width="26.81640625" style="1" customWidth="1"/>
+    <col min="3" max="16384" width="8.90625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" s="3" t="s">
         <v>17</v>
       </c>
       <c r="B1" s="3"/>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
         <v>13</v>
       </c>
@@ -541,7 +541,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
         <v>14</v>
       </c>
@@ -549,7 +549,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A4" s="1" t="s">
         <v>15</v>
       </c>
@@ -557,7 +557,7 @@
         <v>3.1415190000000002</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A5" s="1" t="s">
         <v>16</v>
       </c>
@@ -582,25 +582,25 @@
       <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.90625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="9.5546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="23.88671875" style="1" customWidth="1"/>
-    <col min="3" max="16384" width="8.88671875" style="1"/>
+    <col min="1" max="1" width="9.54296875" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="23.90625" style="1" customWidth="1"/>
+    <col min="3" max="16384" width="8.90625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A3" s="2"/>
       <c r="B3" s="1" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
       <c r="B4" s="1" t="s">
         <v>2</v>
       </c>
@@ -611,7 +611,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
       <c r="B5" s="1" t="s">
         <v>3</v>
       </c>
@@ -622,7 +622,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
       <c r="B6" s="1" t="s">
         <v>4</v>
       </c>
@@ -633,29 +633,29 @@
         <v>10</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
       <c r="B7" s="1" t="s">
         <v>5</v>
       </c>
       <c r="C7" s="1">
-        <v>45</v>
+        <v>54.455593060061851</v>
       </c>
       <c r="D7" s="1" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
       <c r="B8" s="1" t="s">
         <v>6</v>
       </c>
       <c r="C8" s="1">
-        <v>95</v>
+        <v>90</v>
       </c>
       <c r="D8" s="1" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.35">
       <c r="B9" s="1" t="s">
         <v>7</v>
       </c>
@@ -669,7 +669,7 @@
         <v>9.99</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.35">
       <c r="B10" s="1" t="s">
         <v>8</v>
       </c>
@@ -680,18 +680,18 @@
         <v>925.99999999999989</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.35">
       <c r="B11" s="1" t="s">
         <v>18</v>
       </c>
       <c r="C11" s="1">
-        <v>0</v>
+        <v>899.99999999999909</v>
       </c>
       <c r="D11" s="1">
         <v>439.08443537387728</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.35">
       <c r="B12" s="1" t="s">
         <v>19</v>
       </c>
@@ -699,7 +699,7 @@
         <v>865.63897914069571</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.35">
       <c r="B13" s="1" t="s">
         <v>20</v>
       </c>
@@ -707,12 +707,12 @@
         <v>261.00000000000006</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.35">
       <c r="B16" s="1" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="17" spans="2:3" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="2:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B17" s="1" t="s">
         <v>22</v>
       </c>
@@ -720,7 +720,7 @@
         <v>1.2E-2</v>
       </c>
     </row>
-    <row r="18" spans="2:3" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="2:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B18" s="1" t="s">
         <v>23</v>
       </c>
@@ -728,7 +728,7 @@
         <v>0.11</v>
       </c>
     </row>
-    <row r="19" spans="2:3" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="2:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B19" s="1" t="s">
         <v>24</v>
       </c>
@@ -736,12 +736,12 @@
         <v>0.99</v>
       </c>
     </row>
-    <row r="21" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="21" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B21" s="1" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="22" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="22" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B22" s="1" t="s">
         <v>26</v>
       </c>
@@ -749,7 +749,7 @@
         <v>-8350.6714059345395</v>
       </c>
     </row>
-    <row r="23" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="23" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B23" s="1" t="s">
         <v>27</v>
       </c>
@@ -757,7 +757,7 @@
         <v>-48498.809284873329</v>
       </c>
     </row>
-    <row r="24" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="24" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B24" s="1" t="s">
         <v>28</v>
       </c>

</xml_diff>

<commit_message>
test: improve coverage & handling for write_named_range
</commit_message>
<xml_diff>
--- a/tests/xl/datum_excel_tests.xlsx
+++ b/tests/xl/datum_excel_tests.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\blair\datum\tests\xl\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E7500AC3-68E3-4ADD-9BC0-67893599017E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0814CA5D-9A12-4C7C-9E6A-2E8A1E550375}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3040" yWindow="3040" windowWidth="28800" windowHeight="15410" firstSheet="1" activeTab="1" xr2:uid="{4E3D2296-B548-4056-9C4B-8EF4E130383B}"/>
+    <workbookView xWindow="20380" yWindow="1820" windowWidth="16460" windowHeight="15170" xr2:uid="{4E3D2296-B548-4056-9C4B-8EF4E130383B}"/>
   </bookViews>
   <sheets>
     <sheet name="Other Tests" sheetId="3" r:id="rId1"/>
@@ -30,6 +30,7 @@
     <definedName name="HOUSING.moments_of_inertia_centroidal.2">'Gearbox Tests'!$C$19</definedName>
     <definedName name="HOUSING.products_of_inertia_centroidal">'Gearbox Tests'!$C$22:$C$24</definedName>
     <definedName name="missing_ref">'Other Tests'!#REF!</definedName>
+    <definedName name="Range_that_s_too_large">'Other Tests'!$A$7:$H$9</definedName>
     <definedName name="SHAFT_CENTERS">'Gearbox Tests'!$C$10</definedName>
     <definedName name="SHAFT_CENTERS.distance">'Gearbox Tests'!$C$10</definedName>
     <definedName name="SHAFT_CENTERS.point_1.x">'Gearbox Tests'!$C$11</definedName>
@@ -41,6 +42,7 @@
     <definedName name="Test_Int">'Other Tests'!$B$2</definedName>
     <definedName name="Test_Range_1">'Gearbox Tests'!$A$1</definedName>
     <definedName name="Test_Str">'Other Tests'!$B$3</definedName>
+    <definedName name="too_small_range">'Other Tests'!$A$12:$B$12</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -52,7 +54,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="31">
   <si>
     <t>Because spreadsheets need dark mode too!</t>
   </si>
@@ -139,13 +141,19 @@
   </si>
   <si>
     <t>PYZ</t>
+  </si>
+  <si>
+    <t>Range that's too large</t>
+  </si>
+  <si>
+    <t>Range that's too small</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -160,8 +168,16 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="0" tint="-4.9989318521683403E-2"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="4">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -180,6 +196,18 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="-0.499984740745262"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -193,13 +221,16 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="14" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -514,10 +545,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1F223915-F445-4D32-BCC2-8C7735AB3DA4}">
-  <dimension ref="A1:B5"/>
+  <dimension ref="A1:H12"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A7" sqref="A7:H9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.90625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -527,13 +558,13 @@
     <col min="3" max="16384" width="8.90625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A1" s="3" t="s">
         <v>17</v>
       </c>
       <c r="B1" s="3"/>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
         <v>13</v>
       </c>
@@ -541,7 +572,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
         <v>14</v>
       </c>
@@ -549,7 +580,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A4" s="1" t="s">
         <v>15</v>
       </c>
@@ -557,13 +588,51 @@
         <v>3.1415190000000002</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A5" s="1" t="s">
         <v>16</v>
       </c>
       <c r="B5" s="2">
         <v>44682</v>
       </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A7" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="B7" s="4"/>
+      <c r="C7" s="5"/>
+      <c r="D7" s="5"/>
+      <c r="E7" s="5"/>
+      <c r="F7" s="5"/>
+      <c r="G7" s="5"/>
+      <c r="H7" s="5"/>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A8" s="4"/>
+      <c r="B8" s="4"/>
+      <c r="C8" s="5"/>
+      <c r="D8" s="5"/>
+      <c r="E8" s="5"/>
+      <c r="F8" s="5"/>
+      <c r="G8" s="5"/>
+      <c r="H8" s="5"/>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A9" s="4"/>
+      <c r="B9" s="4"/>
+      <c r="C9" s="5"/>
+      <c r="D9" s="5"/>
+      <c r="E9" s="5"/>
+      <c r="F9" s="5"/>
+      <c r="G9" s="5"/>
+      <c r="H9" s="5"/>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A12" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="B12" s="6"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -578,7 +647,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{54907CF9-C14B-4766-B22F-13A5988C480B}">
   <dimension ref="A1:E24"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A6" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+    <sheetView topLeftCell="A6" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
       <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
refactor: Rewrite backup so open workbook isn't closed.
</commit_message>
<xml_diff>
--- a/tests/xl/datum_excel_tests.xlsx
+++ b/tests/xl/datum_excel_tests.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\blair\datum\tests\xl\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0814CA5D-9A12-4C7C-9E6A-2E8A1E550375}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2FCAC470-9774-432F-A71E-C3603B8EA4A4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="20380" yWindow="1820" windowWidth="16460" windowHeight="15170" xr2:uid="{4E3D2296-B548-4056-9C4B-8EF4E130383B}"/>
+    <workbookView xWindow="26720" yWindow="2850" windowWidth="11040" windowHeight="14490" xr2:uid="{4E3D2296-B548-4056-9C4B-8EF4E130383B}"/>
   </bookViews>
   <sheets>
     <sheet name="Other Tests" sheetId="3" r:id="rId1"/>
@@ -225,12 +225,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="14" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -545,10 +545,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1F223915-F445-4D32-BCC2-8C7735AB3DA4}">
-  <dimension ref="A1:H12"/>
+  <dimension ref="A1:O12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A7" sqref="A7:H9"/>
+      <selection activeCell="G5" sqref="G5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.90625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -558,13 +558,13 @@
     <col min="3" max="16384" width="8.90625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A1" s="3" t="s">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A1" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="B1" s="3"/>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="B1" s="6"/>
+    </row>
+    <row r="2" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
         <v>13</v>
       </c>
@@ -572,7 +572,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
         <v>14</v>
       </c>
@@ -580,7 +580,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A4" s="1" t="s">
         <v>15</v>
       </c>
@@ -588,7 +588,7 @@
         <v>3.1415190000000002</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A5" s="1" t="s">
         <v>16</v>
       </c>
@@ -596,43 +596,49 @@
         <v>44682</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A7" s="4" t="s">
+    <row r="7" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A7" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="B7" s="4"/>
-      <c r="C7" s="5"/>
-      <c r="D7" s="5"/>
-      <c r="E7" s="5"/>
-      <c r="F7" s="5"/>
-      <c r="G7" s="5"/>
-      <c r="H7" s="5"/>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A8" s="4"/>
-      <c r="B8" s="4"/>
-      <c r="C8" s="5"/>
-      <c r="D8" s="5"/>
-      <c r="E8" s="5"/>
-      <c r="F8" s="5"/>
-      <c r="G8" s="5"/>
-      <c r="H8" s="5"/>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A9" s="4"/>
-      <c r="B9" s="4"/>
-      <c r="C9" s="5"/>
-      <c r="D9" s="5"/>
-      <c r="E9" s="5"/>
-      <c r="F9" s="5"/>
-      <c r="G9" s="5"/>
-      <c r="H9" s="5"/>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A12" s="6" t="s">
+      <c r="B7" s="3"/>
+      <c r="C7" s="4"/>
+      <c r="D7" s="4"/>
+      <c r="E7" s="4"/>
+      <c r="F7" s="4"/>
+      <c r="G7" s="4"/>
+      <c r="H7" s="4"/>
+      <c r="N7" s="1">
+        <v>3</v>
+      </c>
+      <c r="O7" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="8" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A8" s="3"/>
+      <c r="B8" s="3"/>
+      <c r="C8" s="4"/>
+      <c r="D8" s="4"/>
+      <c r="E8" s="4"/>
+      <c r="F8" s="4"/>
+      <c r="G8" s="4"/>
+      <c r="H8" s="4"/>
+    </row>
+    <row r="9" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A9" s="3"/>
+      <c r="B9" s="3"/>
+      <c r="C9" s="4"/>
+      <c r="D9" s="4"/>
+      <c r="E9" s="4"/>
+      <c r="F9" s="4"/>
+      <c r="G9" s="4"/>
+      <c r="H9" s="4"/>
+    </row>
+    <row r="12" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A12" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="B12" s="6"/>
+      <c r="B12" s="5"/>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>

<commit_message>
test: add several test cases to get_workbook_key_value_pairs. Move case out of unittest
</commit_message>
<xml_diff>
--- a/tests/xl/datum_excel_tests.xlsx
+++ b/tests/xl/datum_excel_tests.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\blair\datum\tests\xl\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2FCAC470-9774-432F-A71E-C3603B8EA4A4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D475FCF8-27E2-4E6B-A1C6-E22C9A3CCAAB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="26720" yWindow="2850" windowWidth="11040" windowHeight="14490" xr2:uid="{4E3D2296-B548-4056-9C4B-8EF4E130383B}"/>
+    <workbookView xWindow="1900" yWindow="1900" windowWidth="17440" windowHeight="12410" xr2:uid="{4E3D2296-B548-4056-9C4B-8EF4E130383B}"/>
   </bookViews>
   <sheets>
     <sheet name="Other Tests" sheetId="3" r:id="rId1"/>
@@ -20,6 +20,7 @@
     <definedName name="AIR_NUT.point_1">'Gearbox Tests'!$C$9:$E$9</definedName>
     <definedName name="Date_range">'Gearbox Tests'!$A$3</definedName>
     <definedName name="DIPSTICK.angle">'Gearbox Tests'!$C$8</definedName>
+    <definedName name="Empty_Range">'Other Tests'!$B$6</definedName>
     <definedName name="FASTENERS.mass">'Gearbox Tests'!$C$6</definedName>
     <definedName name="float_range">'Gearbox Tests'!$A$2</definedName>
     <definedName name="GEARS.mass">'Gearbox Tests'!$C$7</definedName>
@@ -30,7 +31,7 @@
     <definedName name="HOUSING.moments_of_inertia_centroidal.2">'Gearbox Tests'!$C$19</definedName>
     <definedName name="HOUSING.products_of_inertia_centroidal">'Gearbox Tests'!$C$22:$C$24</definedName>
     <definedName name="missing_ref">'Other Tests'!#REF!</definedName>
-    <definedName name="Range_that_s_too_large">'Other Tests'!$A$7:$H$9</definedName>
+    <definedName name="Range_that_s_too_large">'Other Tests'!$A$23:$H$25</definedName>
     <definedName name="SHAFT_CENTERS">'Gearbox Tests'!$C$10</definedName>
     <definedName name="SHAFT_CENTERS.distance">'Gearbox Tests'!$C$10</definedName>
     <definedName name="SHAFT_CENTERS.point_1.x">'Gearbox Tests'!$C$11</definedName>
@@ -38,11 +39,16 @@
     <definedName name="SHAFT_CENTERS.point_1.z">'Gearbox Tests'!$C$13</definedName>
     <definedName name="SURFACE_PAINTED.area">'Gearbox Tests'!$C$4</definedName>
     <definedName name="Test_Date">'Other Tests'!$B$5</definedName>
+    <definedName name="Test_Empty_List">'Other Tests'!$B$10:$D$10</definedName>
+    <definedName name="Test_Empty_Matrix">'Other Tests'!$B$11:$D$13</definedName>
     <definedName name="Test_Float">'Other Tests'!$B$4</definedName>
     <definedName name="Test_Int">'Other Tests'!$B$2</definedName>
+    <definedName name="Test_List">'Other Tests'!$B$7:$D$7</definedName>
+    <definedName name="Test_Matrix">'Other Tests'!$B$7:$D$9</definedName>
     <definedName name="Test_Range_1">'Gearbox Tests'!$A$1</definedName>
     <definedName name="Test_Str">'Other Tests'!$B$3</definedName>
-    <definedName name="too_small_range">'Other Tests'!$A$12:$B$12</definedName>
+    <definedName name="Test_Vector">'Other Tests'!$B$14:$B$16</definedName>
+    <definedName name="too_small_range">'Other Tests'!$A$28:$B$28</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -54,7 +60,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="37">
   <si>
     <t>Because spreadsheets need dark mode too!</t>
   </si>
@@ -147,6 +153,24 @@
   </si>
   <si>
     <t>Range that's too small</t>
+  </si>
+  <si>
+    <t>Test List</t>
+  </si>
+  <si>
+    <t>Test Empty Range, Single Cell</t>
+  </si>
+  <si>
+    <t>Test Empty List</t>
+  </si>
+  <si>
+    <t>Test Matrix</t>
+  </si>
+  <si>
+    <t>Test Empty Matrix</t>
+  </si>
+  <si>
+    <t>Test Vector</t>
   </si>
 </sst>
 </file>
@@ -177,7 +201,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="9">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -208,8 +232,26 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF002060"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="-0.499984740745262"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -217,11 +259,26 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="14" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
@@ -231,6 +288,14 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -545,26 +610,26 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1F223915-F445-4D32-BCC2-8C7735AB3DA4}">
-  <dimension ref="A1:O12"/>
+  <dimension ref="A1:O28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G5" sqref="G5"/>
+      <selection activeCell="B16" sqref="B14:B16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.90625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="8.90625" style="1"/>
-    <col min="2" max="2" width="26.81640625" style="1" customWidth="1"/>
+    <col min="1" max="1" width="15.54296875" style="1" customWidth="1"/>
+    <col min="2" max="2" width="12.08984375" style="1" customWidth="1"/>
     <col min="3" max="16384" width="8.90625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A1" s="6" t="s">
         <v>17</v>
       </c>
       <c r="B1" s="6"/>
     </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
         <v>13</v>
       </c>
@@ -572,7 +637,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
         <v>14</v>
       </c>
@@ -580,7 +645,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A4" s="1" t="s">
         <v>15</v>
       </c>
@@ -588,7 +653,7 @@
         <v>3.1415190000000002</v>
       </c>
     </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A5" s="1" t="s">
         <v>16</v>
       </c>
@@ -596,53 +661,145 @@
         <v>44682</v>
       </c>
     </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.35">
-      <c r="A7" s="3" t="s">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A6" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="B6" s="2"/>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A7" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="B7" s="9">
+        <v>1</v>
+      </c>
+      <c r="C7" s="9">
+        <v>2</v>
+      </c>
+      <c r="D7" s="9">
+        <v>3</v>
+      </c>
+      <c r="E7" s="11" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="B8" s="10">
+        <v>4</v>
+      </c>
+      <c r="C8" s="10">
+        <v>5</v>
+      </c>
+      <c r="D8" s="10">
+        <v>6</v>
+      </c>
+      <c r="E8" s="11"/>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="B9" s="10">
+        <v>7</v>
+      </c>
+      <c r="C9" s="10">
+        <v>8</v>
+      </c>
+      <c r="D9" s="10">
+        <v>9</v>
+      </c>
+      <c r="E9" s="11"/>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A10" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="B10" s="7"/>
+      <c r="C10" s="7"/>
+      <c r="D10" s="7"/>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A11" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="B11" s="12"/>
+      <c r="C11" s="12"/>
+      <c r="D11" s="12"/>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="B12" s="12"/>
+      <c r="C12" s="12"/>
+      <c r="D12" s="12"/>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="B13" s="12"/>
+      <c r="C13" s="12"/>
+      <c r="D13" s="12"/>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A14" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="B14" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="B15" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="B16" s="1">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="23" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A23" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="B7" s="3"/>
-      <c r="C7" s="4"/>
-      <c r="D7" s="4"/>
-      <c r="E7" s="4"/>
-      <c r="F7" s="4"/>
-      <c r="G7" s="4"/>
-      <c r="H7" s="4"/>
-      <c r="N7" s="1">
+      <c r="B23" s="3"/>
+      <c r="C23" s="4"/>
+      <c r="D23" s="4"/>
+      <c r="E23" s="4"/>
+      <c r="F23" s="4"/>
+      <c r="G23" s="4"/>
+      <c r="H23" s="4"/>
+      <c r="N23" s="1">
         <v>3</v>
       </c>
-      <c r="O7" s="1">
+      <c r="O23" s="1">
         <v>4</v>
       </c>
     </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.35">
-      <c r="A8" s="3"/>
-      <c r="B8" s="3"/>
-      <c r="C8" s="4"/>
-      <c r="D8" s="4"/>
-      <c r="E8" s="4"/>
-      <c r="F8" s="4"/>
-      <c r="G8" s="4"/>
-      <c r="H8" s="4"/>
-    </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.35">
-      <c r="A9" s="3"/>
-      <c r="B9" s="3"/>
-      <c r="C9" s="4"/>
-      <c r="D9" s="4"/>
-      <c r="E9" s="4"/>
-      <c r="F9" s="4"/>
-      <c r="G9" s="4"/>
-      <c r="H9" s="4"/>
-    </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.35">
-      <c r="A12" s="5" t="s">
+    <row r="24" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A24" s="3"/>
+      <c r="B24" s="3"/>
+      <c r="C24" s="4"/>
+      <c r="D24" s="4"/>
+      <c r="E24" s="4"/>
+      <c r="F24" s="4"/>
+      <c r="G24" s="4"/>
+      <c r="H24" s="4"/>
+    </row>
+    <row r="25" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A25" s="3"/>
+      <c r="B25" s="3"/>
+      <c r="C25" s="4"/>
+      <c r="D25" s="4"/>
+      <c r="E25" s="4"/>
+      <c r="F25" s="4"/>
+      <c r="G25" s="4"/>
+      <c r="H25" s="4"/>
+    </row>
+    <row r="28" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A28" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="B12" s="5"/>
+      <c r="B28" s="5"/>
     </row>
   </sheetData>
-  <mergeCells count="1">
+  <mergeCells count="2">
     <mergeCell ref="A1:B1"/>
+    <mergeCell ref="E7:E9"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>

</xml_diff>

<commit_message>
test: finished tests for write_named range. All tests passing, and they run an order of magnitude than they did before. All unittest references removed. 100% coverage that I feel good about achieved.
</commit_message>
<xml_diff>
--- a/tests/xl/datum_excel_tests.xlsx
+++ b/tests/xl/datum_excel_tests.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\blair\datum\tests\xl\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D475FCF8-27E2-4E6B-A1C6-E22C9A3CCAAB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C40F3F49-D260-4855-BCC4-7F57F5BFDF9F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1900" yWindow="1900" windowWidth="17440" windowHeight="12410" xr2:uid="{4E3D2296-B548-4056-9C4B-8EF4E130383B}"/>
   </bookViews>
@@ -30,8 +30,9 @@
     <definedName name="HOUSING.moments_of_inertia_centroidal.1">'Gearbox Tests'!$C$18</definedName>
     <definedName name="HOUSING.moments_of_inertia_centroidal.2">'Gearbox Tests'!$C$19</definedName>
     <definedName name="HOUSING.products_of_inertia_centroidal">'Gearbox Tests'!$C$22:$C$24</definedName>
+    <definedName name="List_Test">'Other Tests'!$B$20:$D$20</definedName>
+    <definedName name="Matrix_Test">'Other Tests'!$B$21:$D$23</definedName>
     <definedName name="missing_ref">'Other Tests'!#REF!</definedName>
-    <definedName name="Range_that_s_too_large">'Other Tests'!$A$23:$H$25</definedName>
     <definedName name="SHAFT_CENTERS">'Gearbox Tests'!$C$10</definedName>
     <definedName name="SHAFT_CENTERS.distance">'Gearbox Tests'!$C$10</definedName>
     <definedName name="SHAFT_CENTERS.point_1.x">'Gearbox Tests'!$C$11</definedName>
@@ -46,8 +47,10 @@
     <definedName name="Test_List">'Other Tests'!$B$7:$D$7</definedName>
     <definedName name="Test_Matrix">'Other Tests'!$B$7:$D$9</definedName>
     <definedName name="Test_Range_1">'Gearbox Tests'!$A$1</definedName>
+    <definedName name="Test_Single_Value">'Other Tests'!$B$19</definedName>
     <definedName name="Test_Str">'Other Tests'!$B$3</definedName>
     <definedName name="Test_Vector">'Other Tests'!$B$14:$B$16</definedName>
+    <definedName name="too_large_range">'Other Tests'!$A$24:$C$25</definedName>
     <definedName name="too_small_range">'Other Tests'!$A$28:$B$28</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
@@ -60,7 +63,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="40">
   <si>
     <t>Because spreadsheets need dark mode too!</t>
   </si>
@@ -171,6 +174,15 @@
   </si>
   <si>
     <t>Test Vector</t>
+  </si>
+  <si>
+    <t>Test Single Value</t>
+  </si>
+  <si>
+    <t>List Test</t>
+  </si>
+  <si>
+    <t>Matrix Test</t>
   </si>
 </sst>
 </file>
@@ -201,7 +213,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="9">
+  <fills count="12">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -250,8 +262,26 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="3" tint="-0.499984740745262"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC00000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="3" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -274,11 +304,24 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="14" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
@@ -296,6 +339,9 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -610,10 +656,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1F223915-F445-4D32-BCC2-8C7735AB3DA4}">
-  <dimension ref="A1:O28"/>
+  <dimension ref="A1:E28"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B16" sqref="B14:B16"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="A24" sqref="A24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.90625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -752,45 +798,51 @@
         <v>3</v>
       </c>
     </row>
-    <row r="23" spans="1:15" x14ac:dyDescent="0.35">
-      <c r="A23" s="3" t="s">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A19" s="13" t="s">
+        <v>37</v>
+      </c>
+      <c r="B19" s="13"/>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A20" s="14" t="s">
+        <v>38</v>
+      </c>
+      <c r="B20" s="14"/>
+      <c r="C20" s="14"/>
+      <c r="D20" s="14"/>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A21" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="B21" s="15"/>
+      <c r="C21" s="15"/>
+      <c r="D21" s="15"/>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="B22" s="15"/>
+      <c r="C22" s="15"/>
+      <c r="D22" s="15"/>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="B23" s="15"/>
+      <c r="C23" s="15"/>
+      <c r="D23" s="15"/>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A24" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="B23" s="3"/>
-      <c r="C23" s="4"/>
-      <c r="D23" s="4"/>
-      <c r="E23" s="4"/>
-      <c r="F23" s="4"/>
-      <c r="G23" s="4"/>
-      <c r="H23" s="4"/>
-      <c r="N23" s="1">
-        <v>3</v>
-      </c>
-      <c r="O23" s="1">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="24" spans="1:15" x14ac:dyDescent="0.35">
-      <c r="A24" s="3"/>
       <c r="B24" s="3"/>
       <c r="C24" s="4"/>
-      <c r="D24" s="4"/>
-      <c r="E24" s="4"/>
-      <c r="F24" s="4"/>
-      <c r="G24" s="4"/>
-      <c r="H24" s="4"/>
-    </row>
-    <row r="25" spans="1:15" x14ac:dyDescent="0.35">
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A25" s="3"/>
       <c r="B25" s="3"/>
       <c r="C25" s="4"/>
-      <c r="D25" s="4"/>
-      <c r="E25" s="4"/>
-      <c r="F25" s="4"/>
-      <c r="G25" s="4"/>
-      <c r="H25" s="4"/>
-    </row>
-    <row r="28" spans="1:15" x14ac:dyDescent="0.35">
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A28" s="5" t="s">
         <v>30</v>
       </c>

</xml_diff>